<commit_message>
Changes of 20th june
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/AgentActivity.xlsx
+++ b/NetAgent/src/main/resources/AgentActivity.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c s="4" t="inlineStr" r="D7">
         <is>
-          <t xml:space="preserve">06/07/2022</t>
+          <t xml:space="preserve">06/10/2022</t>
         </is>
       </c>
       <c s="3" t="inlineStr" r="H7">
@@ -489,7 +489,7 @@
       </c>
       <c s="4" t="inlineStr" r="I7">
         <is>
-          <t xml:space="preserve">06/17/2022</t>
+          <t xml:space="preserve">06/20/2022</t>
         </is>
       </c>
     </row>
@@ -1021,6 +1021,18 @@
             </rPr>
             <t xml:space="preserve">PU TM : </t>
           </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">6/17/2022 05:58</t>
+          </r>
         </is>
       </c>
       <c s="15" t="str" r="K24"/>
@@ -1037,6 +1049,18 @@
               <rFont val="Arial"/>
             </rPr>
             <t xml:space="preserve">DEL TM : </t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">6/17/2022 05:59</t>
           </r>
         </is>
       </c>
@@ -1284,6 +1308,18 @@
             </rPr>
             <t xml:space="preserve">PU TM : </t>
           </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">6/17/2022 04:51</t>
+          </r>
         </is>
       </c>
       <c s="15" t="str" r="K32"/>
@@ -1300,6 +1336,18 @@
               <rFont val="Arial"/>
             </rPr>
             <t xml:space="preserve">DEL TM : </t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">6/17/2022 04:51</t>
           </r>
         </is>
       </c>
@@ -1547,6 +1595,18 @@
             </rPr>
             <t xml:space="preserve">PU TM : </t>
           </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">6/17/2022 05:58</t>
+          </r>
         </is>
       </c>
       <c s="15" t="str" r="K40"/>
@@ -1563,6 +1623,18 @@
               <rFont val="Arial"/>
             </rPr>
             <t xml:space="preserve">DEL TM : </t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">6/17/2022 05:58</t>
           </r>
         </is>
       </c>
@@ -1630,7 +1702,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">32396054</t>
+            <t xml:space="preserve">32363688</t>
           </r>
           <r>
             <rPr>
@@ -1654,7 +1726,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">06/17/2022</t>
+            <t xml:space="preserve">04/22/2022</t>
           </r>
         </is>
       </c>
@@ -1663,7 +1735,7 @@
       <c s="12" t="str" r="E43"/>
       <c s="13" t="inlineStr" r="F43">
         <is>
-          <t xml:space="preserve">RAVINA FSL (F5491)</t>
+          <t xml:space="preserve">NOTHING BUNDT CAKES</t>
         </is>
       </c>
       <c s="11" t="str" r="G43"/>
@@ -1673,7 +1745,7 @@
       <c s="12" t="str" r="K43"/>
       <c s="13" t="inlineStr" r="M43">
         <is>
-          <t xml:space="preserve">HENRY</t>
+          <t xml:space="preserve">AUTOMATION COMPANY</t>
         </is>
       </c>
       <c s="12" t="str" r="N43"/>
@@ -1683,13 +1755,13 @@
       <c s="15" t="str" r="E44"/>
       <c s="16" t="inlineStr" r="F44">
         <is>
-          <t xml:space="preserve">304 W BAY AREA BLVD.</t>
+          <t xml:space="preserve">14101 SEELEY AVE.</t>
         </is>
       </c>
       <c s="15" t="str" r="K44"/>
       <c s="16" t="inlineStr" r="M44">
         <is>
-          <t xml:space="preserve">14101 SEELEY AVE.</t>
+          <t xml:space="preserve">194 INTERNATIONAL BLVD.</t>
         </is>
       </c>
       <c s="15" t="str" r="N44"/>
@@ -1711,13 +1783,13 @@
       <c s="15" t="str" r="E46"/>
       <c s="16" t="inlineStr" r="F46">
         <is>
-          <t xml:space="preserve">FONDREN, TX 77598</t>
+          <t xml:space="preserve">BLUE ISLAND, IL 60406</t>
         </is>
       </c>
       <c s="15" t="str" r="K46"/>
       <c s="16" t="inlineStr" r="M46">
         <is>
-          <t xml:space="preserve">BLUE ISLAND, IL 60406</t>
+          <t xml:space="preserve">GLENDALE HEIGHTS, IL 60139</t>
         </is>
       </c>
       <c s="15" t="str" r="N46"/>
@@ -1783,7 +1855,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">150.00</t>
+            <t xml:space="preserve">2.00</t>
           </r>
         </is>
       </c>
@@ -1856,7 +1928,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">3401291</t>
+            <t xml:space="preserve">3368926</t>
           </r>
         </is>
       </c>
@@ -1880,8 +1952,295 @@
       <c s="18" t="str" r="M50"/>
       <c s="20" t="str" r="N50"/>
     </row>
-    <row r="51" ht="18" customHeight="1">
-      <c s="7" t="inlineStr" r="B51">
+    <row r="51" ht="13.7" customHeight="0">
+      <c s="10" t="inlineStr" r="B51">
+        <is>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">32396054</t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve"> / </t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">06/17/2022</t>
+          </r>
+        </is>
+      </c>
+      <c s="11" t="str" r="C51"/>
+      <c s="11" t="str" r="D51"/>
+      <c s="12" t="str" r="E51"/>
+      <c s="13" t="inlineStr" r="F51">
+        <is>
+          <t xml:space="preserve">RAVINA FSL (F5491)</t>
+        </is>
+      </c>
+      <c s="11" t="str" r="G51"/>
+      <c s="11" t="str" r="H51"/>
+      <c s="11" t="str" r="I51"/>
+      <c s="11" t="str" r="J51"/>
+      <c s="12" t="str" r="K51"/>
+      <c s="13" t="inlineStr" r="M51">
+        <is>
+          <t xml:space="preserve">HENRY</t>
+        </is>
+      </c>
+      <c s="12" t="str" r="N51"/>
+    </row>
+    <row r="52" ht="1.8" customHeight="0">
+      <c s="14" t="str" r="B52"/>
+      <c s="15" t="str" r="E52"/>
+      <c s="16" t="inlineStr" r="F52">
+        <is>
+          <t xml:space="preserve">304 W BAY AREA BLVD.</t>
+        </is>
+      </c>
+      <c s="15" t="str" r="K52"/>
+      <c s="16" t="inlineStr" r="M52">
+        <is>
+          <t xml:space="preserve">14101 SEELEY AVE.</t>
+        </is>
+      </c>
+      <c s="15" t="str" r="N52"/>
+    </row>
+    <row r="53" ht="11.85" customHeight="0">
+      <c s="16" t="inlineStr" r="B53">
+        <is>
+          <t xml:space="preserve">PU</t>
+        </is>
+      </c>
+      <c s="15" t="str" r="E53"/>
+      <c s="14" t="str" r="F53"/>
+      <c s="15" t="str" r="K53"/>
+      <c s="14" t="str" r="M53"/>
+      <c s="15" t="str" r="N53"/>
+    </row>
+    <row r="54" ht="3.6" customHeight="0">
+      <c s="14" t="str" r="B54"/>
+      <c s="15" t="str" r="E54"/>
+      <c s="16" t="inlineStr" r="F54">
+        <is>
+          <t xml:space="preserve">FONDREN, TX 77598</t>
+        </is>
+      </c>
+      <c s="15" t="str" r="K54"/>
+      <c s="16" t="inlineStr" r="M54">
+        <is>
+          <t xml:space="preserve">BLUE ISLAND, IL 60406</t>
+        </is>
+      </c>
+      <c s="15" t="str" r="N54"/>
+    </row>
+    <row r="55" ht="10.1" customHeight="0">
+      <c s="17" t="inlineStr" r="B55">
+        <is>
+          <r>
+            <rPr>
+              <b/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">PCS : </t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">1</t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">     </t>
+          </r>
+          <r>
+            <rPr>
+              <b/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">WT : </t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">150.00</t>
+          </r>
+        </is>
+      </c>
+      <c s="15" t="str" r="E55"/>
+      <c s="14" t="str" r="F55"/>
+      <c s="15" t="str" r="K55"/>
+      <c s="14" t="str" r="M55"/>
+      <c s="15" t="str" r="N55"/>
+    </row>
+    <row r="56" ht="5.4" customHeight="0">
+      <c s="14" t="str" r="B56"/>
+      <c s="15" t="str" r="E56"/>
+      <c s="17" t="inlineStr" r="F56">
+        <is>
+          <r>
+            <rPr>
+              <b/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">PU TM : </t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">6/17/2022 04:47</t>
+          </r>
+        </is>
+      </c>
+      <c s="15" t="str" r="K56"/>
+      <c s="17" t="inlineStr" r="M56">
+        <is>
+          <r>
+            <rPr>
+              <b/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">DEL TM : </t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">6/17/2022 04:48</t>
+          </r>
+        </is>
+      </c>
+      <c s="15" t="str" r="N56"/>
+    </row>
+    <row r="57" ht="8.25" customHeight="0">
+      <c s="17" t="inlineStr" r="B57">
+        <is>
+          <r>
+            <rPr>
+              <b/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">PU#   </t>
+          </r>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
+            <t xml:space="preserve">3401291</t>
+          </r>
+        </is>
+      </c>
+      <c s="15" t="str" r="E57"/>
+      <c s="14" t="str" r="F57"/>
+      <c s="15" t="str" r="K57"/>
+      <c s="14" t="str" r="M57"/>
+      <c s="15" t="str" r="N57"/>
+    </row>
+    <row r="58" ht="13.7" customHeight="0">
+      <c s="18" t="str" r="B58"/>
+      <c s="19" t="str" r="C58"/>
+      <c s="19" t="str" r="D58"/>
+      <c s="20" t="str" r="E58"/>
+      <c s="18" t="str" r="F58"/>
+      <c s="19" t="str" r="G58"/>
+      <c s="19" t="str" r="H58"/>
+      <c s="19" t="str" r="I58"/>
+      <c s="19" t="str" r="J58"/>
+      <c s="20" t="str" r="K58"/>
+      <c s="18" t="str" r="M58"/>
+      <c s="20" t="str" r="N58"/>
+    </row>
+    <row r="59" ht="18" customHeight="1">
+      <c s="7" t="inlineStr" r="B59">
         <is>
           <r>
             <rPr>
@@ -1941,7 +2300,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">6</t>
           </r>
           <r>
             <rPr>
@@ -1977,7 +2336,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">6</t>
           </r>
           <r>
             <rPr>
@@ -2013,7 +2372,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">304</t>
+            <t xml:space="preserve">306</t>
           </r>
           <r>
             <rPr>
@@ -2029,21 +2388,21 @@
           </r>
         </is>
       </c>
-      <c s="8" t="str" r="C51"/>
-      <c s="8" t="str" r="D51"/>
-      <c s="8" t="str" r="E51"/>
-      <c s="8" t="str" r="F51"/>
-      <c s="8" t="str" r="G51"/>
-      <c s="8" t="str" r="H51"/>
-      <c s="8" t="str" r="I51"/>
-      <c s="8" t="str" r="J51"/>
-      <c s="8" t="str" r="K51"/>
-      <c s="8" t="str" r="L51"/>
-      <c s="8" t="str" r="M51"/>
-      <c s="9" t="str" r="N51"/>
-    </row>
-    <row r="52" ht="19.45" customHeight="1">
-      <c s="21" t="inlineStr" r="B52">
+      <c s="8" t="str" r="C59"/>
+      <c s="8" t="str" r="D59"/>
+      <c s="8" t="str" r="E59"/>
+      <c s="8" t="str" r="F59"/>
+      <c s="8" t="str" r="G59"/>
+      <c s="8" t="str" r="H59"/>
+      <c s="8" t="str" r="I59"/>
+      <c s="8" t="str" r="J59"/>
+      <c s="8" t="str" r="K59"/>
+      <c s="8" t="str" r="L59"/>
+      <c s="8" t="str" r="M59"/>
+      <c s="9" t="str" r="N59"/>
+    </row>
+    <row r="60" ht="19.45" customHeight="1">
+      <c s="21" t="inlineStr" r="B60">
         <is>
           <r>
             <rPr>
@@ -2103,7 +2462,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">6</t>
           </r>
           <r>
             <rPr>
@@ -2139,7 +2498,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">6</t>
           </r>
           <r>
             <rPr>
@@ -2175,7 +2534,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">304</t>
+            <t xml:space="preserve">306</t>
           </r>
           <r>
             <rPr>
@@ -2192,8 +2551,8 @@
         </is>
       </c>
     </row>
-    <row r="53" ht="0.05" customHeight="1"/>
-    <row r="54" ht="31.7" customHeight="1"/>
+    <row r="61" ht="0.05" customHeight="1"/>
+    <row r="62" ht="31.7" customHeight="1"/>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:D3"/>
@@ -2263,13 +2622,25 @@
     <mergeCell ref="F48:K49"/>
     <mergeCell ref="M48:N49"/>
     <mergeCell ref="B49:E50"/>
-    <mergeCell ref="B51:N51"/>
-    <mergeCell ref="B52:N52"/>
+    <mergeCell ref="B51:E52"/>
+    <mergeCell ref="F51:K51"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="F52:K53"/>
+    <mergeCell ref="M52:N53"/>
+    <mergeCell ref="B53:E54"/>
+    <mergeCell ref="F54:K55"/>
+    <mergeCell ref="M54:N55"/>
+    <mergeCell ref="B55:E56"/>
+    <mergeCell ref="F56:K57"/>
+    <mergeCell ref="M56:N57"/>
+    <mergeCell ref="B57:E58"/>
+    <mergeCell ref="B59:N59"/>
+    <mergeCell ref="B60:N60"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.902079921259843" header="0.25" footer="0.25"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;9 6/17/2022 1:41 AM &amp;C&amp;"Arial,Regular"&amp;9 *Data provided should be considered CONFIDENTIAL and PROPRIETARY* 
+    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;9 6/19/2022 9:44 PM &amp;C&amp;"Arial,Regular"&amp;9 *Data provided should be considered CONFIDENTIAL and PROPRIETARY* 
 &amp;"-,Regular"©2011-2022 MNX Global Logistics. All rights reserved. &amp;R&amp;"Arial,Regular"&amp;9 Print User : automation </oddFooter>
   </headerFooter>
   <drawing r:id="rId7"/>

</xml_diff>

<commit_message>
Changes of 21st June 2022 for Master screens
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/AgentActivity.xlsx
+++ b/NetAgent/src/main/resources/AgentActivity.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c s="4" t="inlineStr" r="D7">
         <is>
-          <t xml:space="preserve">06/10/2022</t>
+          <t xml:space="preserve">06/11/2022</t>
         </is>
       </c>
       <c s="3" t="inlineStr" r="H7">
@@ -489,7 +489,7 @@
       </c>
       <c s="4" t="inlineStr" r="I7">
         <is>
-          <t xml:space="preserve">06/20/2022</t>
+          <t xml:space="preserve">06/21/2022</t>
         </is>
       </c>
     </row>
@@ -2640,7 +2640,7 @@
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.902079921259843" header="0.25" footer="0.25"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;9 6/19/2022 9:44 PM &amp;C&amp;"Arial,Regular"&amp;9 *Data provided should be considered CONFIDENTIAL and PROPRIETARY* 
+    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;9 6/21/2022 12:41 AM &amp;C&amp;"Arial,Regular"&amp;9 *Data provided should be considered CONFIDENTIAL and PROPRIETARY* 
 &amp;"-,Regular"©2011-2022 MNX Global Logistics. All rights reserved. &amp;R&amp;"Arial,Regular"&amp;9 Print User : automation </oddFooter>
   </headerFooter>
   <drawing r:id="rId7"/>

</xml_diff>